<commit_message>
Feat: Resultados de estocástico
</commit_message>
<xml_diff>
--- a/res/percentil.xlsx
+++ b/res/percentil.xlsx
@@ -402,7 +402,7 @@
         <v>2024</v>
       </c>
       <c r="B2">
-        <v>2480</v>
+        <v>2473</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -425,19 +425,19 @@
         <v>2025</v>
       </c>
       <c r="B3">
-        <v>2450.03</v>
+        <v>2440</v>
       </c>
       <c r="C3">
-        <v>35.51499999999999</v>
+        <v>41</v>
       </c>
       <c r="D3">
-        <v>13.505</v>
+        <v>18</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0.4950000000000001</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -448,22 +448,22 @@
         <v>2026</v>
       </c>
       <c r="B4">
-        <v>2414.535</v>
+        <v>2400</v>
       </c>
       <c r="C4">
-        <v>66.51499999999999</v>
+        <v>71</v>
       </c>
       <c r="D4">
-        <v>23.505</v>
+        <v>30</v>
       </c>
       <c r="E4">
-        <v>4.495</v>
+        <v>3</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -471,22 +471,22 @@
         <v>2027</v>
       </c>
       <c r="B5">
-        <v>2377.505</v>
+        <v>2360</v>
       </c>
       <c r="C5">
-        <v>89.51499999999999</v>
+        <v>98</v>
       </c>
       <c r="D5">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="E5">
         <v>6</v>
       </c>
       <c r="F5">
-        <v>4.495</v>
+        <v>4</v>
       </c>
       <c r="G5">
-        <v>4.495</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
@@ -494,22 +494,22 @@
         <v>2028</v>
       </c>
       <c r="B6">
-        <v>2340</v>
+        <v>2320</v>
       </c>
       <c r="C6">
-        <v>109.515</v>
+        <v>121</v>
       </c>
       <c r="D6">
-        <v>40.51499999999999</v>
+        <v>50</v>
       </c>
       <c r="E6">
         <v>9</v>
       </c>
       <c r="F6">
-        <v>6.495</v>
+        <v>7</v>
       </c>
       <c r="G6">
-        <v>6.99</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
@@ -517,22 +517,22 @@
         <v>2029</v>
       </c>
       <c r="B7">
-        <v>2306.505</v>
+        <v>2281</v>
       </c>
       <c r="C7">
-        <v>130.515</v>
+        <v>144</v>
       </c>
       <c r="D7">
-        <v>49.505</v>
+        <v>59</v>
       </c>
       <c r="E7">
-        <v>10.485</v>
+        <v>12</v>
       </c>
       <c r="F7">
-        <v>10.495</v>
+        <v>10</v>
       </c>
       <c r="G7">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8">
@@ -540,22 +540,22 @@
         <v>2030</v>
       </c>
       <c r="B8">
-        <v>2266.505</v>
+        <v>2242</v>
       </c>
       <c r="C8">
-        <v>146.02</v>
+        <v>164</v>
       </c>
       <c r="D8">
-        <v>56.53499999999997</v>
+        <v>67</v>
       </c>
       <c r="E8">
-        <v>15.99</v>
+        <v>15</v>
       </c>
       <c r="F8">
-        <v>10.495</v>
+        <v>13</v>
       </c>
       <c r="G8">
-        <v>13.495</v>
+        <v>19.995</v>
       </c>
     </row>
     <row r="9">
@@ -563,22 +563,22 @@
         <v>2031</v>
       </c>
       <c r="B9">
-        <v>2240.01</v>
+        <v>2204</v>
       </c>
       <c r="C9">
-        <v>164.03</v>
+        <v>184</v>
       </c>
       <c r="D9">
-        <v>64.01999999999998</v>
+        <v>76</v>
       </c>
       <c r="E9">
-        <v>18.495</v>
+        <v>19</v>
       </c>
       <c r="F9">
-        <v>14.485</v>
+        <v>16</v>
       </c>
       <c r="G9">
-        <v>19.99</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10">
@@ -586,22 +586,22 @@
         <v>2032</v>
       </c>
       <c r="B10">
-        <v>2207.525</v>
+        <v>2165</v>
       </c>
       <c r="C10">
-        <v>178</v>
+        <v>202</v>
       </c>
       <c r="D10">
-        <v>69.01999999999998</v>
+        <v>84</v>
       </c>
       <c r="E10">
-        <v>20.99</v>
+        <v>22</v>
       </c>
       <c r="F10">
-        <v>17.485</v>
+        <v>19</v>
       </c>
       <c r="G10">
-        <v>25.99</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11">
@@ -609,22 +609,22 @@
         <v>2033</v>
       </c>
       <c r="B11">
-        <v>2179.01</v>
+        <v>2126</v>
       </c>
       <c r="C11">
-        <v>196.0599999999999</v>
+        <v>220</v>
       </c>
       <c r="D11">
-        <v>79.00999999999999</v>
+        <v>92</v>
       </c>
       <c r="E11">
-        <v>27.495</v>
+        <v>26</v>
       </c>
       <c r="F11">
-        <v>25.495</v>
+        <v>22</v>
       </c>
       <c r="G11">
-        <v>30.99</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -632,22 +632,22 @@
         <v>2034</v>
       </c>
       <c r="B12">
-        <v>2138.02</v>
+        <v>2088</v>
       </c>
       <c r="C12">
-        <v>211.545</v>
+        <v>237</v>
       </c>
       <c r="D12">
-        <v>84.51499999999999</v>
+        <v>100</v>
       </c>
       <c r="E12">
-        <v>30.99</v>
+        <v>30</v>
       </c>
       <c r="F12">
-        <v>28.495</v>
+        <v>26</v>
       </c>
       <c r="G12">
-        <v>35.99</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13">
@@ -655,22 +655,22 @@
         <v>2035</v>
       </c>
       <c r="B13">
-        <v>2102.505</v>
+        <v>2048</v>
       </c>
       <c r="C13">
-        <v>233.03</v>
+        <v>253</v>
       </c>
       <c r="D13">
-        <v>88</v>
+        <v>107</v>
       </c>
       <c r="E13">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F13">
-        <v>33.495</v>
+        <v>29</v>
       </c>
       <c r="G13">
-        <v>40.495</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14">
@@ -678,22 +678,22 @@
         <v>2036</v>
       </c>
       <c r="B14">
-        <v>2071</v>
+        <v>2008</v>
       </c>
       <c r="C14">
-        <v>244.01</v>
+        <v>268</v>
       </c>
       <c r="D14">
-        <v>97.01999999999998</v>
+        <v>115</v>
       </c>
       <c r="E14">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F14">
-        <v>35.495</v>
+        <v>33</v>
       </c>
       <c r="G14">
-        <v>47.99</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15">
@@ -701,22 +701,22 @@
         <v>2037</v>
       </c>
       <c r="B15">
-        <v>2045.585</v>
+        <v>1967</v>
       </c>
       <c r="C15">
-        <v>257.525</v>
+        <v>283</v>
       </c>
       <c r="D15">
-        <v>103.04</v>
+        <v>122</v>
       </c>
       <c r="E15">
-        <v>42.98999999999999</v>
+        <v>41</v>
       </c>
       <c r="F15">
-        <v>42.495</v>
+        <v>36</v>
       </c>
       <c r="G15">
-        <v>58.98999999999999</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16">
@@ -724,22 +724,22 @@
         <v>2038</v>
       </c>
       <c r="B16">
-        <v>1992.505</v>
+        <v>1926</v>
       </c>
       <c r="C16">
-        <v>263.505</v>
+        <v>297</v>
       </c>
       <c r="D16">
-        <v>109.505</v>
+        <v>130</v>
       </c>
       <c r="E16">
-        <v>44.485</v>
+        <v>45</v>
       </c>
       <c r="F16">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G16">
-        <v>68.98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17">
@@ -747,22 +747,22 @@
         <v>2039</v>
       </c>
       <c r="B17">
-        <v>1946.505</v>
+        <v>1884</v>
       </c>
       <c r="C17">
-        <v>277.525</v>
+        <v>310</v>
       </c>
       <c r="D17">
-        <v>114.505</v>
+        <v>137</v>
       </c>
       <c r="E17">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F17">
-        <v>47.485</v>
+        <v>44</v>
       </c>
       <c r="G17">
-        <v>80.495</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18">
@@ -770,22 +770,22 @@
         <v>2040</v>
       </c>
       <c r="B18">
-        <v>1916.555</v>
+        <v>1840</v>
       </c>
       <c r="C18">
-        <v>303.545</v>
+        <v>323</v>
       </c>
       <c r="D18">
-        <v>123.01</v>
+        <v>144</v>
       </c>
       <c r="E18">
-        <v>54.495</v>
+        <v>53</v>
       </c>
       <c r="F18">
-        <v>51.97</v>
+        <v>47.995</v>
       </c>
       <c r="G18">
-        <v>88.97999999999999</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19">
@@ -793,22 +793,22 @@
         <v>2041</v>
       </c>
       <c r="B19">
-        <v>1878.08</v>
+        <v>1796</v>
       </c>
       <c r="C19">
-        <v>312.515</v>
+        <v>335</v>
       </c>
       <c r="D19">
-        <v>124.515</v>
+        <v>151</v>
       </c>
       <c r="E19">
-        <v>57.98999999999999</v>
+        <v>57</v>
       </c>
       <c r="F19">
-        <v>55.495</v>
+        <v>51</v>
       </c>
       <c r="G19">
-        <v>104.495</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20">
@@ -816,22 +816,22 @@
         <v>2042</v>
       </c>
       <c r="B20">
-        <v>1836.14</v>
+        <v>1750</v>
       </c>
       <c r="C20">
-        <v>323.01</v>
+        <v>347</v>
       </c>
       <c r="D20">
-        <v>131.515</v>
+        <v>158</v>
       </c>
       <c r="E20">
-        <v>62.98</v>
+        <v>61</v>
       </c>
       <c r="F20">
-        <v>59.99</v>
+        <v>55</v>
       </c>
       <c r="G20">
-        <v>122.495</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21">
@@ -839,22 +839,22 @@
         <v>2043</v>
       </c>
       <c r="B21">
-        <v>1791.535</v>
+        <v>1703</v>
       </c>
       <c r="C21">
-        <v>326.5649999999999</v>
+        <v>357</v>
       </c>
       <c r="D21">
-        <v>141.03</v>
+        <v>165</v>
       </c>
       <c r="E21">
-        <v>64.98</v>
+        <v>65</v>
       </c>
       <c r="F21">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G21">
-        <v>133.475</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22">
@@ -862,22 +862,22 @@
         <v>2044</v>
       </c>
       <c r="B22">
-        <v>1744.02</v>
+        <v>1654</v>
       </c>
       <c r="C22">
-        <v>331</v>
+        <v>367</v>
       </c>
       <c r="D22">
-        <v>146.525</v>
+        <v>172</v>
       </c>
       <c r="E22">
-        <v>70.485</v>
+        <v>69</v>
       </c>
       <c r="F22">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G22">
-        <v>147.435</v>
+        <v>197</v>
       </c>
     </row>
     <row r="23">
@@ -885,22 +885,22 @@
         <v>2045</v>
       </c>
       <c r="B23">
-        <v>1697.03</v>
+        <v>1604</v>
       </c>
       <c r="C23">
-        <v>345.525</v>
+        <v>377</v>
       </c>
       <c r="D23">
-        <v>155.5549999999999</v>
+        <v>178</v>
       </c>
       <c r="E23">
-        <v>78.99000000000001</v>
+        <v>74</v>
       </c>
       <c r="F23">
-        <v>78.495</v>
+        <v>69</v>
       </c>
       <c r="G23">
-        <v>167.98</v>
+        <v>221</v>
       </c>
     </row>
     <row r="24">
@@ -908,22 +908,22 @@
         <v>2046</v>
       </c>
       <c r="B24">
-        <v>1650.03</v>
+        <v>1552</v>
       </c>
       <c r="C24">
-        <v>365.545</v>
+        <v>386</v>
       </c>
       <c r="D24">
-        <v>162.505</v>
+        <v>185</v>
       </c>
       <c r="E24">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F24">
-        <v>81.495</v>
+        <v>73</v>
       </c>
       <c r="G24">
-        <v>185.445</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25">
@@ -931,22 +931,22 @@
         <v>2047</v>
       </c>
       <c r="B25">
-        <v>1600.02</v>
+        <v>1498</v>
       </c>
       <c r="C25">
-        <v>359.01</v>
+        <v>394</v>
       </c>
       <c r="D25">
-        <v>172.05</v>
+        <v>191</v>
       </c>
       <c r="E25">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F25">
-        <v>92.99000000000001</v>
+        <v>78</v>
       </c>
       <c r="G25">
-        <v>204.93</v>
+        <v>276</v>
       </c>
     </row>
     <row r="26">
@@ -954,22 +954,22 @@
         <v>2048</v>
       </c>
       <c r="B26">
-        <v>1551.03</v>
+        <v>1442</v>
       </c>
       <c r="C26">
-        <v>372.515</v>
+        <v>400</v>
       </c>
       <c r="D26">
-        <v>177.505</v>
+        <v>197</v>
       </c>
       <c r="E26">
-        <v>91.99000000000001</v>
+        <v>87</v>
       </c>
       <c r="F26">
-        <v>101.99</v>
+        <v>84</v>
       </c>
       <c r="G26">
-        <v>233.95</v>
+        <v>307</v>
       </c>
     </row>
     <row r="27">
@@ -977,22 +977,22 @@
         <v>2049</v>
       </c>
       <c r="B27">
-        <v>1489</v>
+        <v>1384</v>
       </c>
       <c r="C27">
-        <v>379.5949999999999</v>
+        <v>406</v>
       </c>
       <c r="D27">
-        <v>185.05</v>
+        <v>203</v>
       </c>
       <c r="E27">
-        <v>100.495</v>
+        <v>92</v>
       </c>
       <c r="F27">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="G27">
-        <v>264</v>
+        <v>341</v>
       </c>
     </row>
     <row r="28">
@@ -1000,22 +1000,22 @@
         <v>2050</v>
       </c>
       <c r="B28">
-        <v>1423.545</v>
+        <v>1325</v>
       </c>
       <c r="C28">
-        <v>374.525</v>
+        <v>410</v>
       </c>
       <c r="D28">
-        <v>186.515</v>
+        <v>209</v>
       </c>
       <c r="E28">
-        <v>103.495</v>
+        <v>96</v>
       </c>
       <c r="F28">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="G28">
-        <v>295.485</v>
+        <v>378</v>
       </c>
     </row>
     <row r="29">
@@ -1023,22 +1023,22 @@
         <v>2051</v>
       </c>
       <c r="B29">
-        <v>1367.01</v>
+        <v>1262</v>
       </c>
       <c r="C29">
-        <v>379.01</v>
+        <v>414</v>
       </c>
       <c r="D29">
-        <v>188.5549999999999</v>
+        <v>214</v>
       </c>
       <c r="E29">
-        <v>110.98</v>
+        <v>101</v>
       </c>
       <c r="F29">
-        <v>130.495</v>
+        <v>102</v>
       </c>
       <c r="G29">
-        <v>332.485</v>
+        <v>419</v>
       </c>
     </row>
     <row r="30">
@@ -1046,22 +1046,22 @@
         <v>2052</v>
       </c>
       <c r="B30">
-        <v>1304.545</v>
+        <v>1198</v>
       </c>
       <c r="C30">
-        <v>388</v>
+        <v>415</v>
       </c>
       <c r="D30">
-        <v>192.02</v>
+        <v>219</v>
       </c>
       <c r="E30">
-        <v>114.485</v>
+        <v>105</v>
       </c>
       <c r="F30">
-        <v>144.455</v>
+        <v>109</v>
       </c>
       <c r="G30">
-        <v>368.97</v>
+        <v>462</v>
       </c>
     </row>
     <row r="31">
@@ -1069,22 +1069,22 @@
         <v>2053</v>
       </c>
       <c r="B31">
-        <v>1228.01</v>
+        <v>1133</v>
       </c>
       <c r="C31">
-        <v>396.02</v>
+        <v>414.0050000000047</v>
       </c>
       <c r="D31">
-        <v>194.01</v>
+        <v>223</v>
       </c>
       <c r="E31">
-        <v>119.485</v>
+        <v>110</v>
       </c>
       <c r="F31">
-        <v>156.99</v>
+        <v>116</v>
       </c>
       <c r="G31">
-        <v>411</v>
+        <v>509</v>
       </c>
     </row>
     <row r="32">
@@ -1092,22 +1092,22 @@
         <v>2054</v>
       </c>
       <c r="B32">
-        <v>1167.03</v>
+        <v>1066</v>
       </c>
       <c r="C32">
-        <v>395</v>
+        <v>412</v>
       </c>
       <c r="D32">
-        <v>204.525</v>
+        <v>227</v>
       </c>
       <c r="E32">
-        <v>124.99</v>
+        <v>114</v>
       </c>
       <c r="F32">
-        <v>168.495</v>
+        <v>125</v>
       </c>
       <c r="G32">
-        <v>445.93</v>
+        <v>560</v>
       </c>
     </row>
     <row r="33">
@@ -1115,22 +1115,22 @@
         <v>2055</v>
       </c>
       <c r="B33">
-        <v>1105.06</v>
+        <v>998</v>
       </c>
       <c r="C33">
-        <v>395.505</v>
+        <v>407</v>
       </c>
       <c r="D33">
-        <v>203.515</v>
+        <v>229</v>
       </c>
       <c r="E33">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="F33">
-        <v>179.465</v>
+        <v>133</v>
       </c>
       <c r="G33">
-        <v>493.92</v>
+        <v>613</v>
       </c>
     </row>
     <row r="34">
@@ -1138,22 +1138,22 @@
         <v>2056</v>
       </c>
       <c r="B34">
-        <v>1027.555</v>
+        <v>929</v>
       </c>
       <c r="C34">
-        <v>381.525</v>
+        <v>401</v>
       </c>
       <c r="D34">
-        <v>207.02</v>
+        <v>230</v>
       </c>
       <c r="E34">
-        <v>129.495</v>
+        <v>122</v>
       </c>
       <c r="F34">
-        <v>194.95</v>
+        <v>141</v>
       </c>
       <c r="G34">
-        <v>547.97</v>
+        <v>671</v>
       </c>
     </row>
     <row r="35">
@@ -1161,22 +1161,22 @@
         <v>2057</v>
       </c>
       <c r="B35">
-        <v>954.6149999999999</v>
+        <v>860</v>
       </c>
       <c r="C35">
-        <v>375</v>
+        <v>392</v>
       </c>
       <c r="D35">
-        <v>215.05</v>
+        <v>231</v>
       </c>
       <c r="E35">
-        <v>137.475</v>
+        <v>125</v>
       </c>
       <c r="F35">
-        <v>212.475</v>
+        <v>150</v>
       </c>
       <c r="G35">
-        <v>608</v>
+        <v>733</v>
       </c>
     </row>
     <row r="36">
@@ -1184,22 +1184,22 @@
         <v>2058</v>
       </c>
       <c r="B36">
-        <v>892.5849999999999</v>
+        <v>792</v>
       </c>
       <c r="C36">
-        <v>372.0699999999999</v>
+        <v>381</v>
       </c>
       <c r="D36">
-        <v>205.515</v>
+        <v>229</v>
       </c>
       <c r="E36">
-        <v>140.475</v>
+        <v>127</v>
       </c>
       <c r="F36">
-        <v>240</v>
+        <v>159</v>
       </c>
       <c r="G36">
-        <v>663.97</v>
+        <v>798</v>
       </c>
     </row>
     <row r="37">
@@ -1207,22 +1207,22 @@
         <v>2059</v>
       </c>
       <c r="B37">
-        <v>827.5749999999999</v>
+        <v>725</v>
       </c>
       <c r="C37">
-        <v>355.535</v>
+        <v>367</v>
       </c>
       <c r="D37">
-        <v>202</v>
+        <v>227</v>
       </c>
       <c r="E37">
-        <v>140.495</v>
+        <v>129</v>
       </c>
       <c r="F37">
-        <v>255.99</v>
+        <v>168</v>
       </c>
       <c r="G37">
-        <v>726.495</v>
+        <v>866</v>
       </c>
     </row>
     <row r="38">
@@ -1230,22 +1230,22 @@
         <v>2060</v>
       </c>
       <c r="B38">
-        <v>754.5649999999999</v>
+        <v>660</v>
       </c>
       <c r="C38">
-        <v>340.0599999999999</v>
+        <v>353</v>
       </c>
       <c r="D38">
-        <v>202.01</v>
+        <v>223</v>
       </c>
       <c r="E38">
-        <v>145.99</v>
+        <v>130</v>
       </c>
       <c r="F38">
-        <v>268.98</v>
+        <v>176</v>
       </c>
       <c r="G38">
-        <v>794.96</v>
+        <v>938</v>
       </c>
     </row>
     <row r="39">
@@ -1253,22 +1253,22 @@
         <v>2061</v>
       </c>
       <c r="B39">
-        <v>677.0799999999999</v>
+        <v>597</v>
       </c>
       <c r="C39">
-        <v>327.5849999999999</v>
+        <v>335</v>
       </c>
       <c r="D39">
-        <v>193.0599999999999</v>
+        <v>217</v>
       </c>
       <c r="E39">
-        <v>145.98</v>
+        <v>129</v>
       </c>
       <c r="F39">
-        <v>288.97</v>
+        <v>184</v>
       </c>
       <c r="G39">
-        <v>864.495</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="40">
@@ -1276,22 +1276,22 @@
         <v>2062</v>
       </c>
       <c r="B40">
-        <v>615.5849999999999</v>
+        <v>536</v>
       </c>
       <c r="C40">
-        <v>303</v>
+        <v>316</v>
       </c>
       <c r="D40">
-        <v>196.01</v>
+        <v>210</v>
       </c>
       <c r="E40">
-        <v>148.99</v>
+        <v>128</v>
       </c>
       <c r="F40">
-        <v>291.94</v>
+        <v>191</v>
       </c>
       <c r="G40">
-        <v>932.97</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="41">
@@ -1299,22 +1299,22 @@
         <v>2063</v>
       </c>
       <c r="B41">
-        <v>548.6249999999999</v>
+        <v>478</v>
       </c>
       <c r="C41">
-        <v>280.05</v>
+        <v>295</v>
       </c>
       <c r="D41">
-        <v>183.02</v>
+        <v>202</v>
       </c>
       <c r="E41">
-        <v>145.485</v>
+        <v>126</v>
       </c>
       <c r="F41">
-        <v>308.97</v>
+        <v>197</v>
       </c>
       <c r="G41">
-        <v>1002.455</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="42">
@@ -1322,22 +1322,22 @@
         <v>2064</v>
       </c>
       <c r="B42">
-        <v>481.5649999999999</v>
+        <v>424</v>
       </c>
       <c r="C42">
-        <v>267.5749999999999</v>
+        <v>273</v>
       </c>
       <c r="D42">
-        <v>175.515</v>
+        <v>192</v>
       </c>
       <c r="E42">
-        <v>139.495</v>
+        <v>123</v>
       </c>
       <c r="F42">
-        <v>323.495</v>
+        <v>201</v>
       </c>
       <c r="G42">
-        <v>1078.405</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="43">
@@ -1345,22 +1345,22 @@
         <v>2065</v>
       </c>
       <c r="B43">
-        <v>420.01</v>
+        <v>373</v>
       </c>
       <c r="C43">
-        <v>241.03</v>
+        <v>251</v>
       </c>
       <c r="D43">
-        <v>162.505</v>
+        <v>181</v>
       </c>
       <c r="E43">
-        <v>130.99</v>
+        <v>119</v>
       </c>
       <c r="F43">
-        <v>322.485</v>
+        <v>204</v>
       </c>
       <c r="G43">
-        <v>1166.95</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="44">
@@ -1368,22 +1368,22 @@
         <v>2066</v>
       </c>
       <c r="B44">
-        <v>373.535</v>
+        <v>326</v>
       </c>
       <c r="C44">
-        <v>213.525</v>
+        <v>228</v>
       </c>
       <c r="D44">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="E44">
-        <v>129.99</v>
+        <v>113</v>
       </c>
       <c r="F44">
-        <v>331.98</v>
+        <v>205</v>
       </c>
       <c r="G44">
-        <v>1251.465</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="45">
@@ -1391,22 +1391,22 @@
         <v>2067</v>
       </c>
       <c r="B45">
-        <v>324.03</v>
+        <v>282</v>
       </c>
       <c r="C45">
-        <v>189.505</v>
+        <v>206</v>
       </c>
       <c r="D45">
-        <v>135.01</v>
+        <v>157</v>
       </c>
       <c r="E45">
-        <v>124.475</v>
+        <v>107</v>
       </c>
       <c r="F45">
-        <v>326</v>
+        <v>205</v>
       </c>
       <c r="G45">
-        <v>1345.475</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="46">
@@ -1414,22 +1414,22 @@
         <v>2068</v>
       </c>
       <c r="B46">
-        <v>282.545</v>
+        <v>243</v>
       </c>
       <c r="C46">
-        <v>170.01</v>
+        <v>184</v>
       </c>
       <c r="D46">
-        <v>130.03</v>
+        <v>144</v>
       </c>
       <c r="E46">
-        <v>120.485</v>
+        <v>100</v>
       </c>
       <c r="F46">
-        <v>317.365</v>
+        <v>202</v>
       </c>
       <c r="G46">
-        <v>1428.495</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="47">
@@ -1437,22 +1437,22 @@
         <v>2069</v>
       </c>
       <c r="B47">
-        <v>239.525</v>
+        <v>208</v>
       </c>
       <c r="C47">
-        <v>153.02</v>
+        <v>162</v>
       </c>
       <c r="D47">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="E47">
-        <v>108.95</v>
+        <v>92</v>
       </c>
       <c r="F47">
-        <v>309.475</v>
+        <v>198</v>
       </c>
       <c r="G47">
-        <v>1513.495</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="48">
@@ -1460,22 +1460,22 @@
         <v>2070</v>
       </c>
       <c r="B48">
-        <v>205.05</v>
+        <v>176</v>
       </c>
       <c r="C48">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="D48">
-        <v>105.01</v>
+        <v>119</v>
       </c>
       <c r="E48">
-        <v>96.485</v>
+        <v>84</v>
       </c>
       <c r="F48">
-        <v>306</v>
+        <v>192</v>
       </c>
       <c r="G48">
-        <v>1595.97</v>
+        <v>1727</v>
       </c>
     </row>
     <row r="49">
@@ -1483,22 +1483,22 @@
         <v>2071</v>
       </c>
       <c r="B49">
-        <v>170.03</v>
+        <v>149</v>
       </c>
       <c r="C49">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="D49">
-        <v>95.05999999999995</v>
+        <v>106</v>
       </c>
       <c r="E49">
-        <v>86.97</v>
+        <v>76</v>
       </c>
       <c r="F49">
-        <v>296.98</v>
+        <v>184</v>
       </c>
       <c r="G49">
-        <v>1679.465</v>
+        <v>1801</v>
       </c>
     </row>
     <row r="50">
@@ -1506,22 +1506,22 @@
         <v>2072</v>
       </c>
       <c r="B50">
-        <v>141.525</v>
+        <v>124</v>
       </c>
       <c r="C50">
-        <v>104.525</v>
+        <v>107</v>
       </c>
       <c r="D50">
-        <v>84.51499999999999</v>
+        <v>94</v>
       </c>
       <c r="E50">
-        <v>73.41500000000001</v>
+        <v>68</v>
       </c>
       <c r="F50">
-        <v>280.95</v>
+        <v>174</v>
       </c>
       <c r="G50">
-        <v>1752.485</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="51">
@@ -1529,22 +1529,22 @@
         <v>2073</v>
       </c>
       <c r="B51">
-        <v>119.525</v>
+        <v>103</v>
       </c>
       <c r="C51">
-        <v>88.505</v>
+        <v>91</v>
       </c>
       <c r="D51">
-        <v>70.00999999999999</v>
+        <v>83</v>
       </c>
       <c r="E51">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F51">
-        <v>263.98</v>
+        <v>163</v>
       </c>
       <c r="G51">
-        <v>1828.495</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="52">
@@ -1552,22 +1552,22 @@
         <v>2074</v>
       </c>
       <c r="B52">
-        <v>96.01999999999998</v>
+        <v>85</v>
       </c>
       <c r="C52">
-        <v>71.53499999999997</v>
+        <v>77</v>
       </c>
       <c r="D52">
-        <v>66.505</v>
+        <v>72</v>
       </c>
       <c r="E52">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F52">
-        <v>240.98</v>
+        <v>151</v>
       </c>
       <c r="G52">
-        <v>1900.98</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="53">
@@ -1575,22 +1575,22 @@
         <v>2075</v>
       </c>
       <c r="B53">
-        <v>80.00999999999999</v>
+        <v>70</v>
       </c>
       <c r="C53">
-        <v>59.00999999999999</v>
+        <v>65</v>
       </c>
       <c r="D53">
-        <v>55.00999999999999</v>
+        <v>62</v>
       </c>
       <c r="E53">
-        <v>51.47499999999999</v>
+        <v>44</v>
       </c>
       <c r="F53">
-        <v>224.485</v>
+        <v>138</v>
       </c>
       <c r="G53">
-        <v>1964.94</v>
+        <v>2056</v>
       </c>
     </row>
     <row r="54">
@@ -1598,22 +1598,22 @@
         <v>2076</v>
       </c>
       <c r="B54">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C54">
-        <v>50.00999999999999</v>
+        <v>54</v>
       </c>
       <c r="D54">
-        <v>46.00999999999999</v>
+        <v>53</v>
       </c>
       <c r="E54">
-        <v>45.495</v>
+        <v>38</v>
       </c>
       <c r="F54">
-        <v>205.495</v>
+        <v>124</v>
       </c>
       <c r="G54">
-        <v>2030.99</v>
+        <v>2109</v>
       </c>
     </row>
     <row r="55">
@@ -1621,22 +1621,22 @@
         <v>2077</v>
       </c>
       <c r="B55">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C55">
-        <v>38.505</v>
+        <v>45</v>
       </c>
       <c r="D55">
-        <v>42.01999999999998</v>
+        <v>45</v>
       </c>
       <c r="E55">
-        <v>37.98999999999999</v>
+        <v>31</v>
       </c>
       <c r="F55">
-        <v>185.98</v>
+        <v>111</v>
       </c>
       <c r="G55">
-        <v>2083.485</v>
+        <v>2157</v>
       </c>
     </row>
     <row r="56">
@@ -1644,22 +1644,22 @@
         <v>2078</v>
       </c>
       <c r="B56">
-        <v>39.01999999999998</v>
+        <v>37</v>
       </c>
       <c r="C56">
-        <v>32.505</v>
+        <v>37</v>
       </c>
       <c r="D56">
-        <v>31.505</v>
+        <v>38</v>
       </c>
       <c r="E56">
-        <v>30.495</v>
+        <v>25</v>
       </c>
       <c r="F56">
-        <v>161.96</v>
+        <v>98</v>
       </c>
       <c r="G56">
-        <v>2134.455</v>
+        <v>2201</v>
       </c>
     </row>
     <row r="57">
@@ -1667,22 +1667,22 @@
         <v>2079</v>
       </c>
       <c r="B57">
+        <v>30</v>
+      </c>
+      <c r="C57">
+        <v>30</v>
+      </c>
+      <c r="D57">
         <v>32</v>
       </c>
-      <c r="C57">
-        <v>27.00999999999999</v>
-      </c>
-      <c r="D57">
-        <v>28.505</v>
-      </c>
       <c r="E57">
-        <v>23.495</v>
+        <v>20</v>
       </c>
       <c r="F57">
-        <v>144.495</v>
+        <v>85</v>
       </c>
       <c r="G57">
-        <v>2184</v>
+        <v>2240</v>
       </c>
     </row>
     <row r="58">
@@ -1690,22 +1690,22 @@
         <v>2080</v>
       </c>
       <c r="B58">
-        <v>27.00999999999999</v>
+        <v>24</v>
       </c>
       <c r="C58">
-        <v>19.505</v>
+        <v>24</v>
       </c>
       <c r="D58">
-        <v>24.00999999999999</v>
+        <v>27</v>
       </c>
       <c r="E58">
-        <v>20.495</v>
+        <v>16</v>
       </c>
       <c r="F58">
-        <v>119.465</v>
+        <v>72</v>
       </c>
       <c r="G58">
-        <v>2225.485</v>
+        <v>2275</v>
       </c>
     </row>
     <row r="59">
@@ -1713,22 +1713,22 @@
         <v>2081</v>
       </c>
       <c r="B59">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C59">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D59">
-        <v>19.00999999999999</v>
+        <v>22</v>
       </c>
       <c r="E59">
-        <v>14.495</v>
+        <v>12</v>
       </c>
       <c r="F59">
-        <v>98.45500000000001</v>
+        <v>61</v>
       </c>
       <c r="G59">
-        <v>2266.485</v>
+        <v>2305</v>
       </c>
     </row>
     <row r="60">
@@ -1736,22 +1736,22 @@
         <v>2082</v>
       </c>
       <c r="B60">
-        <v>15.505</v>
+        <v>15</v>
       </c>
       <c r="C60">
-        <v>14.51499999999999</v>
+        <v>16</v>
       </c>
       <c r="D60">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E60">
-        <v>10.495</v>
+        <v>9</v>
       </c>
       <c r="F60">
-        <v>87.98</v>
+        <v>51</v>
       </c>
       <c r="G60">
-        <v>2299.495</v>
+        <v>2332</v>
       </c>
     </row>
     <row r="61">
@@ -1759,22 +1759,22 @@
         <v>2083</v>
       </c>
       <c r="B61">
-        <v>11.505</v>
+        <v>12</v>
       </c>
       <c r="C61">
-        <v>11.505</v>
+        <v>13</v>
       </c>
       <c r="D61">
-        <v>14.505</v>
+        <v>15</v>
       </c>
       <c r="E61">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F61">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="G61">
-        <v>2330</v>
+        <v>2355</v>
       </c>
     </row>
     <row r="62">
@@ -1782,22 +1782,22 @@
         <v>2084</v>
       </c>
       <c r="B62">
-        <v>9.504999999999995</v>
+        <v>9</v>
       </c>
       <c r="C62">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D62">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E62">
-        <v>4.99</v>
+        <v>4</v>
       </c>
       <c r="F62">
-        <v>56.495</v>
+        <v>34</v>
       </c>
       <c r="G62">
-        <v>2352.485</v>
+        <v>2375</v>
       </c>
     </row>
     <row r="63">
@@ -1805,22 +1805,22 @@
         <v>2085</v>
       </c>
       <c r="B63">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C63">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D63">
-        <v>8.504999999999995</v>
+        <v>11</v>
       </c>
       <c r="E63">
-        <v>3.495</v>
+        <v>3</v>
       </c>
       <c r="F63">
-        <v>45.97</v>
+        <v>26</v>
       </c>
       <c r="G63">
-        <v>2375</v>
+        <v>2392</v>
       </c>
     </row>
     <row r="64">
@@ -1828,22 +1828,22 @@
         <v>2086</v>
       </c>
       <c r="B64">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C64">
-        <v>5.504999999999995</v>
+        <v>7</v>
       </c>
       <c r="D64">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E64">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F64">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="G64">
-        <v>2394.495</v>
+        <v>2406</v>
       </c>
     </row>
     <row r="65">
@@ -1851,22 +1851,22 @@
         <v>2087</v>
       </c>
       <c r="B65">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C65">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D65">
-        <v>7.009999999999991</v>
+        <v>7</v>
       </c>
       <c r="E65">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65">
-        <v>29.495</v>
+        <v>15</v>
       </c>
       <c r="G65">
-        <v>2409.475</v>
+        <v>2418</v>
       </c>
     </row>
     <row r="66">
@@ -1874,22 +1874,22 @@
         <v>2088</v>
       </c>
       <c r="B66">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C66">
-        <v>4.504999999999995</v>
+        <v>4</v>
       </c>
       <c r="D66">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F66">
-        <v>20.495</v>
+        <v>11</v>
       </c>
       <c r="G66">
-        <v>2417.465</v>
+        <v>2428</v>
       </c>
     </row>
     <row r="67">
@@ -1897,22 +1897,22 @@
         <v>2089</v>
       </c>
       <c r="B67">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C67">
-        <v>3.504999999999995</v>
+        <v>4</v>
       </c>
       <c r="D67">
-        <v>5.019999999999982</v>
+        <v>5</v>
       </c>
       <c r="E67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F67">
-        <v>15.495</v>
+        <v>8</v>
       </c>
       <c r="G67">
-        <v>2429.98</v>
+        <v>2436</v>
       </c>
     </row>
     <row r="68">
@@ -1920,10 +1920,10 @@
         <v>2090</v>
       </c>
       <c r="B68">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C68">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D68">
         <v>4</v>
@@ -1932,10 +1932,10 @@
         <v>0</v>
       </c>
       <c r="F68">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G68">
-        <v>2438.99</v>
+        <v>2443</v>
       </c>
     </row>
     <row r="69">
@@ -1943,22 +1943,22 @@
         <v>2091</v>
       </c>
       <c r="B69">
-        <v>1.504999999999995</v>
+        <v>2</v>
       </c>
       <c r="C69">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D69">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E69">
         <v>0</v>
       </c>
       <c r="F69">
-        <v>8.495000000000001</v>
+        <v>3</v>
       </c>
       <c r="G69">
-        <v>2446.99</v>
+        <v>2449</v>
       </c>
     </row>
     <row r="70">
@@ -1969,19 +1969,19 @@
         <v>2</v>
       </c>
       <c r="C70">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D70">
+        <v>3</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
         <v>2</v>
       </c>
-      <c r="E70">
-        <v>0</v>
-      </c>
-      <c r="F70">
-        <v>3.495</v>
-      </c>
       <c r="G70">
-        <v>2453.485</v>
+        <v>2453</v>
       </c>
     </row>
     <row r="71">
@@ -1989,22 +1989,22 @@
         <v>2093</v>
       </c>
       <c r="B71">
-        <v>1.504999999999995</v>
+        <v>1</v>
       </c>
       <c r="C71">
+        <v>2</v>
+      </c>
+      <c r="D71">
+        <v>2</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
         <v>1</v>
       </c>
-      <c r="D71">
-        <v>2.504999999999995</v>
-      </c>
-      <c r="E71">
-        <v>0</v>
-      </c>
-      <c r="F71">
-        <v>2.495</v>
-      </c>
       <c r="G71">
-        <v>2461</v>
+        <v>2457</v>
       </c>
     </row>
     <row r="72">
@@ -2015,19 +2015,19 @@
         <v>1</v>
       </c>
       <c r="C72">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D72">
-        <v>1.504999999999995</v>
+        <v>2</v>
       </c>
       <c r="E72">
         <v>0</v>
       </c>
       <c r="F72">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G72">
-        <v>2463.495</v>
+        <v>2460</v>
       </c>
     </row>
     <row r="73">
@@ -2038,19 +2038,19 @@
         <v>1</v>
       </c>
       <c r="C73">
-        <v>0.5049999999999955</v>
+        <v>1</v>
       </c>
       <c r="D73">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E73">
         <v>0</v>
       </c>
       <c r="F73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G73">
-        <v>2467.495</v>
+        <v>2463</v>
       </c>
     </row>
     <row r="74">
@@ -2061,10 +2061,10 @@
         <v>1</v>
       </c>
       <c r="C74">
-        <v>0.5049999999999955</v>
+        <v>1</v>
       </c>
       <c r="D74">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E74">
         <v>0</v>
@@ -2073,7 +2073,7 @@
         <v>0</v>
       </c>
       <c r="G74">
-        <v>2470.495</v>
+        <v>2465</v>
       </c>
     </row>
     <row r="75">
@@ -2081,10 +2081,10 @@
         <v>2097</v>
       </c>
       <c r="B75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C75">
-        <v>0.5049999999999955</v>
+        <v>1</v>
       </c>
       <c r="D75">
         <v>1</v>
@@ -2096,7 +2096,7 @@
         <v>0</v>
       </c>
       <c r="G75">
-        <v>2472.495</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="76">
@@ -2104,10 +2104,10 @@
         <v>2098</v>
       </c>
       <c r="B76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C76">
-        <v>0.5049999999999955</v>
+        <v>1</v>
       </c>
       <c r="D76">
         <v>1</v>
@@ -2119,7 +2119,7 @@
         <v>0</v>
       </c>
       <c r="G76">
-        <v>2473.495</v>
+        <v>2468</v>
       </c>
     </row>
     <row r="77">
@@ -2127,10 +2127,10 @@
         <v>2099</v>
       </c>
       <c r="B77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D77">
         <v>1</v>
@@ -2142,7 +2142,7 @@
         <v>0</v>
       </c>
       <c r="G77">
-        <v>2474.99</v>
+        <v>2469</v>
       </c>
     </row>
     <row r="78">
@@ -2153,7 +2153,7 @@
         <v>0</v>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D78">
         <v>1</v>
@@ -2165,7 +2165,7 @@
         <v>0</v>
       </c>
       <c r="G78">
-        <v>2476</v>
+        <v>2469</v>
       </c>
     </row>
     <row r="79">
@@ -2176,7 +2176,7 @@
         <v>0</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D79">
         <v>1</v>
@@ -2188,7 +2188,7 @@
         <v>0</v>
       </c>
       <c r="G79">
-        <v>2477</v>
+        <v>2470</v>
       </c>
     </row>
     <row r="80">
@@ -2202,7 +2202,7 @@
         <v>0</v>
       </c>
       <c r="D80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E80">
         <v>0</v>
@@ -2211,7 +2211,7 @@
         <v>0</v>
       </c>
       <c r="G80">
-        <v>2477.495</v>
+        <v>2471</v>
       </c>
     </row>
     <row r="81">
@@ -2225,7 +2225,7 @@
         <v>0</v>
       </c>
       <c r="D81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E81">
         <v>0</v>
@@ -2234,7 +2234,7 @@
         <v>0</v>
       </c>
       <c r="G81">
-        <v>2478</v>
+        <v>2471</v>
       </c>
     </row>
     <row r="82">
@@ -2248,7 +2248,7 @@
         <v>0</v>
       </c>
       <c r="D82">
-        <v>0.5049999999999955</v>
+        <v>0</v>
       </c>
       <c r="E82">
         <v>0</v>
@@ -2257,7 +2257,7 @@
         <v>0</v>
       </c>
       <c r="G82">
-        <v>2479</v>
+        <v>2471</v>
       </c>
     </row>
     <row r="83">
@@ -2271,7 +2271,7 @@
         <v>0</v>
       </c>
       <c r="D83">
-        <v>0.5049999999999955</v>
+        <v>0</v>
       </c>
       <c r="E83">
         <v>0</v>
@@ -2280,7 +2280,7 @@
         <v>0</v>
       </c>
       <c r="G83">
-        <v>2479</v>
+        <v>2472</v>
       </c>
     </row>
     <row r="84">
@@ -2294,7 +2294,7 @@
         <v>0</v>
       </c>
       <c r="D84">
-        <v>0.5049999999999955</v>
+        <v>0</v>
       </c>
       <c r="E84">
         <v>0</v>
@@ -2303,7 +2303,7 @@
         <v>0</v>
       </c>
       <c r="G84">
-        <v>2479</v>
+        <v>2472</v>
       </c>
     </row>
     <row r="85">
@@ -2317,7 +2317,7 @@
         <v>0</v>
       </c>
       <c r="D85">
-        <v>0.5049999999999955</v>
+        <v>0</v>
       </c>
       <c r="E85">
         <v>0</v>
@@ -2326,7 +2326,7 @@
         <v>0</v>
       </c>
       <c r="G85">
-        <v>2479</v>
+        <v>2472</v>
       </c>
     </row>
     <row r="86">
@@ -2349,7 +2349,7 @@
         <v>0</v>
       </c>
       <c r="G86">
-        <v>2479</v>
+        <v>2472</v>
       </c>
     </row>
     <row r="87">
@@ -2372,7 +2372,7 @@
         <v>0</v>
       </c>
       <c r="G87">
-        <v>2479.495</v>
+        <v>2472</v>
       </c>
     </row>
     <row r="88">
@@ -2395,7 +2395,7 @@
         <v>0</v>
       </c>
       <c r="G88">
-        <v>2479.495</v>
+        <v>2472</v>
       </c>
     </row>
     <row r="89">
@@ -2418,7 +2418,7 @@
         <v>0</v>
       </c>
       <c r="G89">
-        <v>2480</v>
+        <v>2473</v>
       </c>
     </row>
     <row r="90">
@@ -2441,7 +2441,7 @@
         <v>0</v>
       </c>
       <c r="G90">
-        <v>2480</v>
+        <v>2473</v>
       </c>
     </row>
     <row r="91">
@@ -2464,7 +2464,7 @@
         <v>0</v>
       </c>
       <c r="G91">
-        <v>2480</v>
+        <v>2473</v>
       </c>
     </row>
     <row r="92">
@@ -2487,7 +2487,7 @@
         <v>0</v>
       </c>
       <c r="G92">
-        <v>2480</v>
+        <v>2473</v>
       </c>
     </row>
     <row r="93">
@@ -2510,7 +2510,7 @@
         <v>0</v>
       </c>
       <c r="G93">
-        <v>2480</v>
+        <v>2473</v>
       </c>
     </row>
     <row r="94">
@@ -2533,7 +2533,7 @@
         <v>0</v>
       </c>
       <c r="G94">
-        <v>2480</v>
+        <v>2473</v>
       </c>
     </row>
     <row r="95">
@@ -2556,7 +2556,7 @@
         <v>0</v>
       </c>
       <c r="G95">
-        <v>2480</v>
+        <v>2473</v>
       </c>
     </row>
     <row r="96">
@@ -2579,7 +2579,7 @@
         <v>0</v>
       </c>
       <c r="G96">
-        <v>2480</v>
+        <v>2473</v>
       </c>
     </row>
     <row r="97">
@@ -2602,7 +2602,7 @@
         <v>0</v>
       </c>
       <c r="G97">
-        <v>2480</v>
+        <v>2473</v>
       </c>
     </row>
     <row r="98">
@@ -2625,7 +2625,7 @@
         <v>0</v>
       </c>
       <c r="G98">
-        <v>2480</v>
+        <v>2473</v>
       </c>
     </row>
     <row r="99">
@@ -2648,7 +2648,7 @@
         <v>0</v>
       </c>
       <c r="G99">
-        <v>2480</v>
+        <v>2473</v>
       </c>
     </row>
     <row r="100">
@@ -2671,7 +2671,7 @@
         <v>0</v>
       </c>
       <c r="G100">
-        <v>2480</v>
+        <v>2473</v>
       </c>
     </row>
     <row r="101">
@@ -2694,7 +2694,7 @@
         <v>0</v>
       </c>
       <c r="G101">
-        <v>2480</v>
+        <v>2473</v>
       </c>
     </row>
     <row r="102">
@@ -2717,7 +2717,7 @@
         <v>0</v>
       </c>
       <c r="G102">
-        <v>2480</v>
+        <v>2473</v>
       </c>
     </row>
   </sheetData>
@@ -2775,7 +2775,7 @@
         <v>2024</v>
       </c>
       <c r="B2">
-        <v>2520</v>
+        <v>2527</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -2798,22 +2798,22 @@
         <v>2025</v>
       </c>
       <c r="B3">
-        <v>2491.505</v>
+        <v>2501</v>
       </c>
       <c r="C3">
-        <v>40.02999999999997</v>
+        <v>36</v>
       </c>
       <c r="D3">
-        <v>13.00999999999999</v>
+        <v>13</v>
       </c>
       <c r="E3">
-        <v>0.4950000000000001</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0.4950000000000001</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>0.4950000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -2821,22 +2821,22 @@
         <v>2026</v>
       </c>
       <c r="B4">
-        <v>2451.01</v>
+        <v>2469</v>
       </c>
       <c r="C4">
-        <v>64.505</v>
+        <v>62</v>
       </c>
       <c r="D4">
-        <v>23.00999999999999</v>
+        <v>22</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4">
-        <v>3.495</v>
+        <v>2</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -2844,22 +2844,22 @@
         <v>2027</v>
       </c>
       <c r="B5">
-        <v>2411.505</v>
+        <v>2436</v>
       </c>
       <c r="C5">
-        <v>87.00999999999999</v>
+        <v>85</v>
       </c>
       <c r="D5">
-        <v>33.505</v>
+        <v>30</v>
       </c>
       <c r="E5">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F5">
-        <v>5.495</v>
+        <v>5</v>
       </c>
       <c r="G5">
-        <v>4.495</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -2867,22 +2867,22 @@
         <v>2028</v>
       </c>
       <c r="B6">
-        <v>2374.02</v>
+        <v>2404</v>
       </c>
       <c r="C6">
-        <v>114.02</v>
+        <v>106</v>
       </c>
       <c r="D6">
-        <v>47.00999999999999</v>
+        <v>37</v>
       </c>
       <c r="E6">
-        <v>10.495</v>
+        <v>8</v>
       </c>
       <c r="F6">
-        <v>9.495000000000001</v>
+        <v>8</v>
       </c>
       <c r="G6">
-        <v>9.495000000000001</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -2890,22 +2890,22 @@
         <v>2029</v>
       </c>
       <c r="B7">
-        <v>2330.505</v>
+        <v>2372</v>
       </c>
       <c r="C7">
-        <v>132.0599999999999</v>
+        <v>125</v>
       </c>
       <c r="D7">
-        <v>55.53499999999997</v>
+        <v>43</v>
       </c>
       <c r="E7">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F7">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G7">
-        <v>14.495</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
@@ -2913,22 +2913,22 @@
         <v>2030</v>
       </c>
       <c r="B8">
-        <v>2298.01</v>
+        <v>2340</v>
       </c>
       <c r="C8">
-        <v>150.515</v>
+        <v>143</v>
       </c>
       <c r="D8">
-        <v>64.53499999999997</v>
+        <v>50</v>
       </c>
       <c r="E8">
-        <v>16.99</v>
+        <v>14</v>
       </c>
       <c r="F8">
-        <v>16.485</v>
+        <v>14</v>
       </c>
       <c r="G8">
-        <v>19.495</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
@@ -2936,22 +2936,22 @@
         <v>2031</v>
       </c>
       <c r="B9">
-        <v>2260.545</v>
+        <v>2308</v>
       </c>
       <c r="C9">
-        <v>176.02</v>
+        <v>160</v>
       </c>
       <c r="D9">
-        <v>68.01999999999998</v>
+        <v>57</v>
       </c>
       <c r="E9">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F9">
-        <v>20.495</v>
+        <v>18</v>
       </c>
       <c r="G9">
-        <v>23.99</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10">
@@ -2959,22 +2959,22 @@
         <v>2032</v>
       </c>
       <c r="B10">
-        <v>2224.515</v>
+        <v>2276</v>
       </c>
       <c r="C10">
-        <v>191.01</v>
+        <v>175</v>
       </c>
       <c r="D10">
-        <v>71.51499999999999</v>
+        <v>63</v>
       </c>
       <c r="E10">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F10">
-        <v>21.98</v>
+        <v>21</v>
       </c>
       <c r="G10">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11">
@@ -2982,22 +2982,22 @@
         <v>2033</v>
       </c>
       <c r="B11">
-        <v>2193.585</v>
+        <v>2244</v>
       </c>
       <c r="C11">
-        <v>203.525</v>
+        <v>191</v>
       </c>
       <c r="D11">
-        <v>81.00999999999999</v>
+        <v>69</v>
       </c>
       <c r="E11">
-        <v>26.495</v>
+        <v>25</v>
       </c>
       <c r="F11">
-        <v>25.99</v>
+        <v>25</v>
       </c>
       <c r="G11">
-        <v>35.495</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12">
@@ -3005,22 +3005,22 @@
         <v>2034</v>
       </c>
       <c r="B12">
-        <v>2154.635</v>
+        <v>2211</v>
       </c>
       <c r="C12">
-        <v>213.01</v>
+        <v>206</v>
       </c>
       <c r="D12">
-        <v>89.505</v>
+        <v>75</v>
       </c>
       <c r="E12">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F12">
-        <v>27.98</v>
+        <v>28</v>
       </c>
       <c r="G12">
-        <v>40.98</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13">
@@ -3028,22 +3028,22 @@
         <v>2035</v>
       </c>
       <c r="B13">
-        <v>2121.1</v>
+        <v>2177</v>
       </c>
       <c r="C13">
-        <v>237.505</v>
+        <v>221</v>
       </c>
       <c r="D13">
-        <v>96.00999999999999</v>
+        <v>82</v>
       </c>
       <c r="E13">
-        <v>34.97</v>
+        <v>32</v>
       </c>
       <c r="F13">
-        <v>30.99</v>
+        <v>32</v>
       </c>
       <c r="G13">
-        <v>48.99</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14">
@@ -3051,22 +3051,22 @@
         <v>2036</v>
       </c>
       <c r="B14">
-        <v>2080.555</v>
+        <v>2143</v>
       </c>
       <c r="C14">
-        <v>258.535</v>
+        <v>235</v>
       </c>
       <c r="D14">
-        <v>102.505</v>
+        <v>88</v>
       </c>
       <c r="E14">
-        <v>35.98</v>
+        <v>36</v>
       </c>
       <c r="F14">
-        <v>35.485</v>
+        <v>36</v>
       </c>
       <c r="G14">
-        <v>56.465</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15">
@@ -3074,22 +3074,22 @@
         <v>2037</v>
       </c>
       <c r="B15">
-        <v>2030.505</v>
+        <v>2108</v>
       </c>
       <c r="C15">
-        <v>270.03</v>
+        <v>249</v>
       </c>
       <c r="D15">
-        <v>106.01</v>
+        <v>95</v>
       </c>
       <c r="E15">
-        <v>38.95</v>
+        <v>40</v>
       </c>
       <c r="F15">
-        <v>39.455</v>
+        <v>41</v>
       </c>
       <c r="G15">
-        <v>70</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16">
@@ -3097,22 +3097,22 @@
         <v>2038</v>
       </c>
       <c r="B16">
-        <v>1999.02</v>
+        <v>2072</v>
       </c>
       <c r="C16">
-        <v>281.525</v>
+        <v>263</v>
       </c>
       <c r="D16">
-        <v>115.01</v>
+        <v>101</v>
       </c>
       <c r="E16">
-        <v>43.95</v>
+        <v>44</v>
       </c>
       <c r="F16">
-        <v>47.495</v>
+        <v>45</v>
       </c>
       <c r="G16">
-        <v>77.99000000000001</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17">
@@ -3120,22 +3120,22 @@
         <v>2039</v>
       </c>
       <c r="B17">
-        <v>1950.02</v>
+        <v>2035</v>
       </c>
       <c r="C17">
-        <v>304.525</v>
+        <v>276</v>
       </c>
       <c r="D17">
-        <v>121.505</v>
+        <v>107</v>
       </c>
       <c r="E17">
-        <v>44.94</v>
+        <v>49</v>
       </c>
       <c r="F17">
         <v>50</v>
       </c>
       <c r="G17">
-        <v>88.96000000000001</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18">
@@ -3143,22 +3143,22 @@
         <v>2040</v>
       </c>
       <c r="B18">
-        <v>1917.04</v>
+        <v>1997</v>
       </c>
       <c r="C18">
-        <v>309</v>
+        <v>288</v>
       </c>
       <c r="D18">
-        <v>136.03</v>
+        <v>114</v>
       </c>
       <c r="E18">
-        <v>50.435</v>
+        <v>53</v>
       </c>
       <c r="F18">
-        <v>51.99</v>
+        <v>55</v>
       </c>
       <c r="G18">
-        <v>102.98</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19">
@@ -3166,22 +3166,22 @@
         <v>2041</v>
       </c>
       <c r="B19">
-        <v>1859.01</v>
+        <v>1957</v>
       </c>
       <c r="C19">
-        <v>315.525</v>
+        <v>301</v>
       </c>
       <c r="D19">
-        <v>134.505</v>
+        <v>120</v>
       </c>
       <c r="E19">
-        <v>56.485</v>
+        <v>58</v>
       </c>
       <c r="F19">
-        <v>58.98</v>
+        <v>60</v>
       </c>
       <c r="G19">
-        <v>119.465</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20">
@@ -3189,22 +3189,22 @@
         <v>2042</v>
       </c>
       <c r="B20">
-        <v>1826.07</v>
+        <v>1916</v>
       </c>
       <c r="C20">
-        <v>321.01</v>
+        <v>314</v>
       </c>
       <c r="D20">
-        <v>147.02</v>
+        <v>127</v>
       </c>
       <c r="E20">
-        <v>64.98</v>
+        <v>63</v>
       </c>
       <c r="F20">
-        <v>64.485</v>
+        <v>66</v>
       </c>
       <c r="G20">
-        <v>134</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21">
@@ -3212,22 +3212,22 @@
         <v>2043</v>
       </c>
       <c r="B21">
-        <v>1780.03</v>
+        <v>1873</v>
       </c>
       <c r="C21">
-        <v>342.04</v>
+        <v>325</v>
       </c>
       <c r="D21">
-        <v>150.505</v>
+        <v>133</v>
       </c>
       <c r="E21">
-        <v>71.98999999999999</v>
+        <v>68</v>
       </c>
       <c r="F21">
-        <v>69.485</v>
+        <v>72</v>
       </c>
       <c r="G21">
-        <v>153.475</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22">
@@ -3235,22 +3235,22 @@
         <v>2044</v>
       </c>
       <c r="B22">
-        <v>1727.06</v>
+        <v>1829</v>
       </c>
       <c r="C22">
-        <v>352</v>
+        <v>335</v>
       </c>
       <c r="D22">
-        <v>161.515</v>
+        <v>140</v>
       </c>
       <c r="E22">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F22">
-        <v>75.485</v>
+        <v>79</v>
       </c>
       <c r="G22">
-        <v>177</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23">
@@ -3258,22 +3258,22 @@
         <v>2045</v>
       </c>
       <c r="B23">
-        <v>1679.515</v>
+        <v>1783</v>
       </c>
       <c r="C23">
-        <v>355.505</v>
+        <v>345</v>
       </c>
       <c r="D23">
-        <v>164.03</v>
+        <v>146</v>
       </c>
       <c r="E23">
-        <v>78.47499999999999</v>
+        <v>78</v>
       </c>
       <c r="F23">
-        <v>82.98</v>
+        <v>87</v>
       </c>
       <c r="G23">
-        <v>196</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24">
@@ -3281,22 +3281,22 @@
         <v>2046</v>
       </c>
       <c r="B24">
-        <v>1632.06</v>
+        <v>1734</v>
       </c>
       <c r="C24">
-        <v>369</v>
+        <v>355</v>
       </c>
       <c r="D24">
-        <v>175.02</v>
+        <v>152</v>
       </c>
       <c r="E24">
-        <v>85.47499999999999</v>
+        <v>84</v>
       </c>
       <c r="F24">
-        <v>90.98</v>
+        <v>95</v>
       </c>
       <c r="G24">
-        <v>215.465</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25">
@@ -3304,22 +3304,22 @@
         <v>2047</v>
       </c>
       <c r="B25">
-        <v>1594.12</v>
+        <v>1682</v>
       </c>
       <c r="C25">
-        <v>375.515</v>
+        <v>363</v>
       </c>
       <c r="D25">
-        <v>173.01</v>
+        <v>159</v>
       </c>
       <c r="E25">
-        <v>88.99000000000001</v>
+        <v>90</v>
       </c>
       <c r="F25">
-        <v>97.99000000000001</v>
+        <v>105</v>
       </c>
       <c r="G25">
-        <v>246.99</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26">
@@ -3327,22 +3327,22 @@
         <v>2048</v>
       </c>
       <c r="B26">
-        <v>1526.605</v>
+        <v>1629</v>
       </c>
       <c r="C26">
-        <v>379.505</v>
+        <v>371</v>
       </c>
       <c r="D26">
-        <v>183</v>
+        <v>165</v>
       </c>
       <c r="E26">
-        <v>98.99000000000001</v>
+        <v>96</v>
       </c>
       <c r="F26">
-        <v>103.99</v>
+        <v>115</v>
       </c>
       <c r="G26">
-        <v>277.99</v>
+        <v>193</v>
       </c>
     </row>
     <row r="27">
@@ -3350,22 +3350,22 @@
         <v>2049</v>
       </c>
       <c r="B27">
-        <v>1460.1</v>
+        <v>1572</v>
       </c>
       <c r="C27">
-        <v>392.01</v>
+        <v>378</v>
       </c>
       <c r="D27">
-        <v>187.505</v>
+        <v>171</v>
       </c>
       <c r="E27">
-        <v>102.465</v>
+        <v>102</v>
       </c>
       <c r="F27">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="G27">
-        <v>305.485</v>
+        <v>217</v>
       </c>
     </row>
     <row r="28">
@@ -3373,22 +3373,22 @@
         <v>2050</v>
       </c>
       <c r="B28">
-        <v>1396.01</v>
+        <v>1512</v>
       </c>
       <c r="C28">
-        <v>402.6349999999999</v>
+        <v>383</v>
       </c>
       <c r="D28">
-        <v>194.515</v>
+        <v>177</v>
       </c>
       <c r="E28">
-        <v>111.475</v>
+        <v>109</v>
       </c>
       <c r="F28">
-        <v>124.99</v>
+        <v>140</v>
       </c>
       <c r="G28">
-        <v>338.99</v>
+        <v>243</v>
       </c>
     </row>
     <row r="29">
@@ -3396,22 +3396,22 @@
         <v>2051</v>
       </c>
       <c r="B29">
-        <v>1334.02</v>
+        <v>1448</v>
       </c>
       <c r="C29">
-        <v>399.03</v>
+        <v>388</v>
       </c>
       <c r="D29">
-        <v>202.515</v>
+        <v>182</v>
       </c>
       <c r="E29">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="F29">
-        <v>133.99</v>
+        <v>155</v>
       </c>
       <c r="G29">
-        <v>372.435</v>
+        <v>273</v>
       </c>
     </row>
     <row r="30">
@@ -3419,22 +3419,22 @@
         <v>2052</v>
       </c>
       <c r="B30">
-        <v>1263.05</v>
+        <v>1381</v>
       </c>
       <c r="C30">
-        <v>411.545</v>
+        <v>389</v>
       </c>
       <c r="D30">
-        <v>204.0599999999999</v>
+        <v>188</v>
       </c>
       <c r="E30">
-        <v>124.455</v>
+        <v>123</v>
       </c>
       <c r="F30">
-        <v>146</v>
+        <v>172</v>
       </c>
       <c r="G30">
-        <v>409.415</v>
+        <v>305</v>
       </c>
     </row>
     <row r="31">
@@ -3442,22 +3442,22 @@
         <v>2053</v>
       </c>
       <c r="B31">
-        <v>1203.525</v>
+        <v>1312</v>
       </c>
       <c r="C31">
-        <v>398.0599999999999</v>
+        <v>390</v>
       </c>
       <c r="D31">
-        <v>202.01</v>
+        <v>192</v>
       </c>
       <c r="E31">
-        <v>126.98</v>
+        <v>130</v>
       </c>
       <c r="F31">
-        <v>151</v>
+        <v>189</v>
       </c>
       <c r="G31">
-        <v>451.455</v>
+        <v>341</v>
       </c>
     </row>
     <row r="32">
@@ -3465,22 +3465,22 @@
         <v>2054</v>
       </c>
       <c r="B32">
-        <v>1120.565</v>
+        <v>1240</v>
       </c>
       <c r="C32">
-        <v>395.02</v>
+        <v>388</v>
       </c>
       <c r="D32">
-        <v>207.505</v>
+        <v>196</v>
       </c>
       <c r="E32">
-        <v>135.99</v>
+        <v>136</v>
       </c>
       <c r="F32">
-        <v>170.97</v>
+        <v>209</v>
       </c>
       <c r="G32">
-        <v>498.95</v>
+        <v>381</v>
       </c>
     </row>
     <row r="33">
@@ -3488,22 +3488,22 @@
         <v>2055</v>
       </c>
       <c r="B33">
-        <v>1045.01</v>
+        <v>1165</v>
       </c>
       <c r="C33">
-        <v>393.0699999999999</v>
+        <v>384</v>
       </c>
       <c r="D33">
-        <v>212.5649999999999</v>
+        <v>198</v>
       </c>
       <c r="E33">
-        <v>138.465</v>
+        <v>143</v>
       </c>
       <c r="F33">
-        <v>186.485</v>
+        <v>230</v>
       </c>
       <c r="G33">
-        <v>552.485</v>
+        <v>425</v>
       </c>
     </row>
     <row r="34">
@@ -3511,22 +3511,22 @@
         <v>2056</v>
       </c>
       <c r="B34">
-        <v>978.525</v>
+        <v>1090</v>
       </c>
       <c r="C34">
-        <v>381.02</v>
+        <v>378</v>
       </c>
       <c r="D34">
-        <v>214.515</v>
+        <v>199</v>
       </c>
       <c r="E34">
-        <v>141.98</v>
+        <v>149</v>
       </c>
       <c r="F34">
-        <v>196.98</v>
+        <v>253</v>
       </c>
       <c r="G34">
-        <v>607.99</v>
+        <v>472</v>
       </c>
     </row>
     <row r="35">
@@ -3534,22 +3534,22 @@
         <v>2057</v>
       </c>
       <c r="B35">
-        <v>907.01</v>
+        <v>1014</v>
       </c>
       <c r="C35">
-        <v>376.505</v>
+        <v>368</v>
       </c>
       <c r="D35">
-        <v>212.01</v>
+        <v>200</v>
       </c>
       <c r="E35">
-        <v>143.98</v>
+        <v>154</v>
       </c>
       <c r="F35">
-        <v>222.465</v>
+        <v>276</v>
       </c>
       <c r="G35">
-        <v>672.98</v>
+        <v>525</v>
       </c>
     </row>
     <row r="36">
@@ -3557,22 +3557,22 @@
         <v>2058</v>
       </c>
       <c r="B36">
-        <v>837.515</v>
+        <v>936</v>
       </c>
       <c r="C36">
-        <v>368.515</v>
+        <v>356</v>
       </c>
       <c r="D36">
-        <v>214.02</v>
+        <v>198</v>
       </c>
       <c r="E36">
-        <v>147.96</v>
+        <v>158</v>
       </c>
       <c r="F36">
-        <v>234.475</v>
+        <v>299</v>
       </c>
       <c r="G36">
-        <v>738.475</v>
+        <v>582</v>
       </c>
     </row>
     <row r="37">
@@ -3580,22 +3580,22 @@
         <v>2059</v>
       </c>
       <c r="B37">
-        <v>772.505</v>
+        <v>861</v>
       </c>
       <c r="C37">
-        <v>354.5549999999999</v>
+        <v>342</v>
       </c>
       <c r="D37">
-        <v>213.0699999999999</v>
+        <v>196</v>
       </c>
       <c r="E37">
-        <v>150.475</v>
+        <v>161</v>
       </c>
       <c r="F37">
-        <v>250.495</v>
+        <v>323</v>
       </c>
       <c r="G37">
-        <v>802.485</v>
+        <v>644</v>
       </c>
     </row>
     <row r="38">
@@ -3603,22 +3603,22 @@
         <v>2060</v>
       </c>
       <c r="B38">
-        <v>701.0599999999999</v>
+        <v>785</v>
       </c>
       <c r="C38">
-        <v>335.01</v>
+        <v>326</v>
       </c>
       <c r="D38">
-        <v>204.505</v>
+        <v>191</v>
       </c>
       <c r="E38">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="F38">
-        <v>254.435</v>
+        <v>346</v>
       </c>
       <c r="G38">
-        <v>871.96</v>
+        <v>710</v>
       </c>
     </row>
     <row r="39">
@@ -3626,22 +3626,22 @@
         <v>2061</v>
       </c>
       <c r="B39">
-        <v>627.5749999999999</v>
+        <v>712</v>
       </c>
       <c r="C39">
-        <v>315.02</v>
+        <v>308</v>
       </c>
       <c r="D39">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="E39">
-        <v>151.99</v>
+        <v>162</v>
       </c>
       <c r="F39">
-        <v>272.425</v>
+        <v>369</v>
       </c>
       <c r="G39">
-        <v>949</v>
+        <v>781</v>
       </c>
     </row>
     <row r="40">
@@ -3649,22 +3649,22 @@
         <v>2062</v>
       </c>
       <c r="B40">
-        <v>562.0799999999999</v>
+        <v>640</v>
       </c>
       <c r="C40">
-        <v>300.515</v>
+        <v>288</v>
       </c>
       <c r="D40">
-        <v>192.01</v>
+        <v>178</v>
       </c>
       <c r="E40">
-        <v>147.485</v>
+        <v>160</v>
       </c>
       <c r="F40">
-        <v>282.455</v>
+        <v>388</v>
       </c>
       <c r="G40">
-        <v>1031.99</v>
+        <v>856</v>
       </c>
     </row>
     <row r="41">
@@ -3672,22 +3672,22 @@
         <v>2063</v>
       </c>
       <c r="B41">
-        <v>510.02</v>
+        <v>572</v>
       </c>
       <c r="C41">
-        <v>279.04</v>
+        <v>267</v>
       </c>
       <c r="D41">
-        <v>181.525</v>
+        <v>170</v>
       </c>
       <c r="E41">
-        <v>137.445</v>
+        <v>156</v>
       </c>
       <c r="F41">
-        <v>302.99</v>
+        <v>405</v>
       </c>
       <c r="G41">
-        <v>1106.475</v>
+        <v>935</v>
       </c>
     </row>
     <row r="42">
@@ -3695,22 +3695,22 @@
         <v>2064</v>
       </c>
       <c r="B42">
-        <v>438.515</v>
+        <v>507</v>
       </c>
       <c r="C42">
-        <v>255.515</v>
+        <v>244</v>
       </c>
       <c r="D42">
-        <v>173.545</v>
+        <v>160</v>
       </c>
       <c r="E42">
-        <v>138.99</v>
+        <v>151</v>
       </c>
       <c r="F42">
-        <v>313.99</v>
+        <v>419</v>
       </c>
       <c r="G42">
-        <v>1200.98</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="43">
@@ -3718,22 +3718,22 @@
         <v>2065</v>
       </c>
       <c r="B43">
-        <v>391.03</v>
+        <v>447</v>
       </c>
       <c r="C43">
-        <v>232.5749999999999</v>
+        <v>222</v>
       </c>
       <c r="D43">
-        <v>156.505</v>
+        <v>150</v>
       </c>
       <c r="E43">
-        <v>130.455</v>
+        <v>145</v>
       </c>
       <c r="F43">
-        <v>318.485</v>
+        <v>428</v>
       </c>
       <c r="G43">
-        <v>1280.465</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="44">
@@ -3741,22 +3741,22 @@
         <v>2066</v>
       </c>
       <c r="B44">
-        <v>331</v>
+        <v>390</v>
       </c>
       <c r="C44">
-        <v>210.5649999999999</v>
+        <v>200</v>
       </c>
       <c r="D44">
-        <v>147.02</v>
+        <v>139</v>
       </c>
       <c r="E44">
-        <v>122.455</v>
+        <v>136</v>
       </c>
       <c r="F44">
-        <v>322.485</v>
+        <v>433</v>
       </c>
       <c r="G44">
-        <v>1361.475</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="45">
@@ -3764,22 +3764,22 @@
         <v>2067</v>
       </c>
       <c r="B45">
-        <v>287.515</v>
+        <v>338</v>
       </c>
       <c r="C45">
-        <v>180.505</v>
+        <v>178</v>
       </c>
       <c r="D45">
-        <v>142.02</v>
+        <v>127</v>
       </c>
       <c r="E45">
-        <v>118.495</v>
+        <v>127</v>
       </c>
       <c r="F45">
-        <v>319.96</v>
+        <v>433</v>
       </c>
       <c r="G45">
-        <v>1455.495</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="46">
@@ -3787,22 +3787,22 @@
         <v>2068</v>
       </c>
       <c r="B46">
-        <v>246.505</v>
+        <v>290</v>
       </c>
       <c r="C46">
-        <v>159.01</v>
+        <v>158</v>
       </c>
       <c r="D46">
-        <v>121.525</v>
+        <v>115</v>
       </c>
       <c r="E46">
-        <v>106.495</v>
+        <v>118</v>
       </c>
       <c r="F46">
-        <v>319.495</v>
+        <v>429</v>
       </c>
       <c r="G46">
-        <v>1543</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="47">
@@ -3810,22 +3810,22 @@
         <v>2069</v>
       </c>
       <c r="B47">
-        <v>216.535</v>
+        <v>248</v>
       </c>
       <c r="C47">
-        <v>140.535</v>
+        <v>138</v>
       </c>
       <c r="D47">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="E47">
-        <v>99.97</v>
+        <v>107.995</v>
       </c>
       <c r="F47">
-        <v>305.98</v>
+        <v>419</v>
       </c>
       <c r="G47">
-        <v>1616.96</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="48">
@@ -3833,22 +3833,22 @@
         <v>2070</v>
       </c>
       <c r="B48">
-        <v>179.505</v>
+        <v>210</v>
       </c>
       <c r="C48">
-        <v>121.01</v>
+        <v>120</v>
       </c>
       <c r="D48">
-        <v>105.515</v>
+        <v>93</v>
       </c>
       <c r="E48">
-        <v>90.495</v>
+        <v>97</v>
       </c>
       <c r="F48">
-        <v>301.97</v>
+        <v>405</v>
       </c>
       <c r="G48">
-        <v>1704.495</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="49">
@@ -3856,22 +3856,22 @@
         <v>2071</v>
       </c>
       <c r="B49">
-        <v>160.525</v>
+        <v>176</v>
       </c>
       <c r="C49">
-        <v>104.505</v>
+        <v>103</v>
       </c>
       <c r="D49">
-        <v>90.53499999999997</v>
+        <v>82</v>
       </c>
       <c r="E49">
-        <v>77.99000000000001</v>
+        <v>86</v>
       </c>
       <c r="F49">
-        <v>284.9299999999999</v>
+        <v>387</v>
       </c>
       <c r="G49">
-        <v>1782.99</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="50">
@@ -3879,22 +3879,22 @@
         <v>2072</v>
       </c>
       <c r="B50">
-        <v>128.05</v>
+        <v>147</v>
       </c>
       <c r="C50">
-        <v>89.505</v>
+        <v>88</v>
       </c>
       <c r="D50">
-        <v>78.53499999999997</v>
+        <v>72</v>
       </c>
       <c r="E50">
-        <v>72.495</v>
+        <v>76</v>
       </c>
       <c r="F50">
-        <v>269.98</v>
+        <v>365</v>
       </c>
       <c r="G50">
-        <v>1863.495</v>
+        <v>1723</v>
       </c>
     </row>
     <row r="51">
@@ -3902,22 +3902,22 @@
         <v>2073</v>
       </c>
       <c r="B51">
-        <v>102.505</v>
+        <v>121</v>
       </c>
       <c r="C51">
-        <v>77.00999999999999</v>
+        <v>74</v>
       </c>
       <c r="D51">
-        <v>68.505</v>
+        <v>63</v>
       </c>
       <c r="E51">
-        <v>58.94</v>
+        <v>66</v>
       </c>
       <c r="F51">
-        <v>250.495</v>
+        <v>340</v>
       </c>
       <c r="G51">
-        <v>1932.485</v>
+        <v>1805</v>
       </c>
     </row>
     <row r="52">
@@ -3925,22 +3925,22 @@
         <v>2074</v>
       </c>
       <c r="B52">
-        <v>85.02999999999997</v>
+        <v>100</v>
       </c>
       <c r="C52">
-        <v>63.505</v>
+        <v>62</v>
       </c>
       <c r="D52">
+        <v>54</v>
+      </c>
+      <c r="E52">
         <v>56</v>
       </c>
-      <c r="E52">
-        <v>48.98</v>
-      </c>
       <c r="F52">
-        <v>223.495</v>
+        <v>314</v>
       </c>
       <c r="G52">
-        <v>2002.95</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="53">
@@ -3948,22 +3948,22 @@
         <v>2075</v>
       </c>
       <c r="B53">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="C53">
-        <v>53.53499999999997</v>
+        <v>52</v>
       </c>
       <c r="D53">
-        <v>51.51499999999999</v>
+        <v>46</v>
       </c>
       <c r="E53">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F53">
-        <v>194.485</v>
+        <v>286</v>
       </c>
       <c r="G53">
-        <v>2069.495</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="54">
@@ -3971,22 +3971,22 @@
         <v>2076</v>
       </c>
       <c r="B54">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="C54">
-        <v>43.00999999999999</v>
+        <v>43</v>
       </c>
       <c r="D54">
-        <v>42.00999999999999</v>
+        <v>39</v>
       </c>
       <c r="E54">
-        <v>37.98999999999999</v>
+        <v>39</v>
       </c>
       <c r="F54">
-        <v>172.99</v>
+        <v>258</v>
       </c>
       <c r="G54">
-        <v>2126.495</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="55">
@@ -3994,22 +3994,22 @@
         <v>2077</v>
       </c>
       <c r="B55">
-        <v>43.00999999999999</v>
+        <v>53</v>
       </c>
       <c r="C55">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D55">
-        <v>35.505</v>
+        <v>33</v>
       </c>
       <c r="E55">
-        <v>33.495</v>
+        <v>32</v>
       </c>
       <c r="F55">
-        <v>152.98</v>
+        <v>229</v>
       </c>
       <c r="G55">
-        <v>2173.99</v>
+        <v>2088</v>
       </c>
     </row>
     <row r="56">
@@ -4017,22 +4017,22 @@
         <v>2078</v>
       </c>
       <c r="B56">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C56">
-        <v>28.51499999999999</v>
+        <v>29</v>
       </c>
       <c r="D56">
-        <v>27.00999999999999</v>
+        <v>28</v>
       </c>
       <c r="E56">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F56">
-        <v>137.99</v>
+        <v>201.995</v>
       </c>
       <c r="G56">
-        <v>2219.99</v>
+        <v>2146</v>
       </c>
     </row>
     <row r="57">
@@ -4040,22 +4040,22 @@
         <v>2079</v>
       </c>
       <c r="B57">
-        <v>25.505</v>
+        <v>34</v>
       </c>
       <c r="C57">
-        <v>23.00999999999999</v>
+        <v>23</v>
       </c>
       <c r="D57">
-        <v>21.505</v>
+        <v>23</v>
       </c>
       <c r="E57">
         <v>20</v>
       </c>
       <c r="F57">
-        <v>122.97</v>
+        <v>175</v>
       </c>
       <c r="G57">
-        <v>2262.485</v>
+        <v>2199</v>
       </c>
     </row>
     <row r="58">
@@ -4063,22 +4063,22 @@
         <v>2080</v>
       </c>
       <c r="B58">
-        <v>22.51499999999999</v>
+        <v>27</v>
       </c>
       <c r="C58">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D58">
-        <v>19.51499999999999</v>
+        <v>20</v>
       </c>
       <c r="E58">
         <v>16</v>
       </c>
       <c r="F58">
-        <v>104.98</v>
+        <v>150</v>
       </c>
       <c r="G58">
-        <v>2300.98</v>
+        <v>2246</v>
       </c>
     </row>
     <row r="59">
@@ -4086,22 +4086,22 @@
         <v>2081</v>
       </c>
       <c r="B59">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C59">
-        <v>15.505</v>
+        <v>15</v>
       </c>
       <c r="D59">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E59">
-        <v>11.495</v>
+        <v>12</v>
       </c>
       <c r="F59">
-        <v>87.47499999999999</v>
+        <v>127</v>
       </c>
       <c r="G59">
-        <v>2337.98</v>
+        <v>2289</v>
       </c>
     </row>
     <row r="60">
@@ -4109,22 +4109,22 @@
         <v>2082</v>
       </c>
       <c r="B60">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C60">
-        <v>12.00999999999999</v>
+        <v>12</v>
       </c>
       <c r="D60">
-        <v>14.00999999999999</v>
+        <v>13</v>
       </c>
       <c r="E60">
-        <v>9.495000000000001</v>
+        <v>9</v>
       </c>
       <c r="F60">
-        <v>73.99000000000001</v>
+        <v>106</v>
       </c>
       <c r="G60">
-        <v>2361.94</v>
+        <v>2326</v>
       </c>
     </row>
     <row r="61">
@@ -4135,19 +4135,19 @@
         <v>13</v>
       </c>
       <c r="C61">
-        <v>9.504999999999995</v>
+        <v>10</v>
       </c>
       <c r="D61">
-        <v>11.505</v>
+        <v>11</v>
       </c>
       <c r="E61">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F61">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="G61">
-        <v>2386.98</v>
+        <v>2358</v>
       </c>
     </row>
     <row r="62">
@@ -4155,22 +4155,22 @@
         <v>2084</v>
       </c>
       <c r="B62">
-        <v>10.505</v>
+        <v>11</v>
       </c>
       <c r="C62">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D62">
-        <v>8.504999999999995</v>
+        <v>9</v>
       </c>
       <c r="E62">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F62">
-        <v>47.485</v>
+        <v>70</v>
       </c>
       <c r="G62">
-        <v>2410.475</v>
+        <v>2386</v>
       </c>
     </row>
     <row r="63">
@@ -4178,22 +4178,22 @@
         <v>2085</v>
       </c>
       <c r="B63">
-        <v>6.504999999999995</v>
+        <v>8</v>
       </c>
       <c r="C63">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D63">
-        <v>7.504999999999995</v>
+        <v>8</v>
       </c>
       <c r="E63">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F63">
-        <v>36.485</v>
+        <v>56</v>
       </c>
       <c r="G63">
-        <v>2431</v>
+        <v>2410</v>
       </c>
     </row>
     <row r="64">
@@ -4201,22 +4201,22 @@
         <v>2086</v>
       </c>
       <c r="B64">
+        <v>7</v>
+      </c>
+      <c r="C64">
+        <v>5</v>
+      </c>
+      <c r="D64">
         <v>6</v>
       </c>
-      <c r="C64">
-        <v>5.504999999999995</v>
-      </c>
-      <c r="D64">
-        <v>6.504999999999995</v>
-      </c>
       <c r="E64">
-        <v>0.4950000000000001</v>
+        <v>1</v>
       </c>
       <c r="F64">
-        <v>27.99</v>
+        <v>44</v>
       </c>
       <c r="G64">
-        <v>2447.475</v>
+        <v>2431</v>
       </c>
     </row>
     <row r="65">
@@ -4227,19 +4227,19 @@
         <v>5</v>
       </c>
       <c r="C65">
-        <v>5.504999999999995</v>
+        <v>4</v>
       </c>
       <c r="D65">
         <v>5</v>
       </c>
       <c r="E65">
-        <v>0.4950000000000001</v>
+        <v>1</v>
       </c>
       <c r="F65">
-        <v>21.98</v>
+        <v>34</v>
       </c>
       <c r="G65">
-        <v>2458.495</v>
+        <v>2448</v>
       </c>
     </row>
     <row r="66">
@@ -4247,22 +4247,22 @@
         <v>2088</v>
       </c>
       <c r="B66">
-        <v>3.504999999999995</v>
+        <v>4</v>
       </c>
       <c r="C66">
         <v>4</v>
       </c>
       <c r="D66">
-        <v>5.504999999999995</v>
+        <v>4</v>
       </c>
       <c r="E66">
-        <v>0.4950000000000001</v>
+        <v>0</v>
       </c>
       <c r="F66">
-        <v>16.475</v>
+        <v>25</v>
       </c>
       <c r="G66">
-        <v>2471</v>
+        <v>2463</v>
       </c>
     </row>
     <row r="67">
@@ -4270,22 +4270,22 @@
         <v>2089</v>
       </c>
       <c r="B67">
+        <v>4</v>
+      </c>
+      <c r="C67">
         <v>3</v>
-      </c>
-      <c r="C67">
-        <v>4.009999999999991</v>
       </c>
       <c r="D67">
         <v>4</v>
       </c>
       <c r="E67">
-        <v>0.4950000000000001</v>
+        <v>0</v>
       </c>
       <c r="F67">
-        <v>11.495</v>
+        <v>19</v>
       </c>
       <c r="G67">
-        <v>2480</v>
+        <v>2475</v>
       </c>
     </row>
     <row r="68">
@@ -4296,7 +4296,7 @@
         <v>3</v>
       </c>
       <c r="C68">
-        <v>2.504999999999995</v>
+        <v>3</v>
       </c>
       <c r="D68">
         <v>3</v>
@@ -4305,10 +4305,10 @@
         <v>0</v>
       </c>
       <c r="F68">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G68">
-        <v>2487.495</v>
+        <v>2485</v>
       </c>
     </row>
     <row r="69">
@@ -4322,16 +4322,16 @@
         <v>2</v>
       </c>
       <c r="D69">
-        <v>3.009999999999991</v>
+        <v>3</v>
       </c>
       <c r="E69">
         <v>0</v>
       </c>
       <c r="F69">
-        <v>6.495</v>
+        <v>9</v>
       </c>
       <c r="G69">
-        <v>2494.495</v>
+        <v>2493</v>
       </c>
     </row>
     <row r="70">
@@ -4339,22 +4339,22 @@
         <v>2092</v>
       </c>
       <c r="B70">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C70">
-        <v>2.504999999999995</v>
+        <v>2</v>
       </c>
       <c r="D70">
-        <v>2.504999999999995</v>
+        <v>2</v>
       </c>
       <c r="E70">
         <v>0</v>
       </c>
       <c r="F70">
-        <v>4.495</v>
+        <v>6</v>
       </c>
       <c r="G70">
-        <v>2497.99</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="71">
@@ -4362,10 +4362,10 @@
         <v>2093</v>
       </c>
       <c r="B71">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C71">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D71">
         <v>2</v>
@@ -4374,10 +4374,10 @@
         <v>0</v>
       </c>
       <c r="F71">
-        <v>3.495</v>
+        <v>4</v>
       </c>
       <c r="G71">
-        <v>2501.99</v>
+        <v>2505</v>
       </c>
     </row>
     <row r="72">
@@ -4388,19 +4388,19 @@
         <v>1</v>
       </c>
       <c r="C72">
+        <v>1</v>
+      </c>
+      <c r="D72">
         <v>2</v>
       </c>
-      <c r="D72">
-        <v>1</v>
-      </c>
       <c r="E72">
         <v>0</v>
       </c>
       <c r="F72">
-        <v>2.495</v>
+        <v>2</v>
       </c>
       <c r="G72">
-        <v>2505.495</v>
+        <v>2509</v>
       </c>
     </row>
     <row r="73">
@@ -4420,10 +4420,10 @@
         <v>0</v>
       </c>
       <c r="F73">
-        <v>0.4950000000000001</v>
+        <v>1</v>
       </c>
       <c r="G73">
-        <v>2509</v>
+        <v>2513</v>
       </c>
     </row>
     <row r="74">
@@ -4437,7 +4437,7 @@
         <v>1</v>
       </c>
       <c r="D74">
-        <v>1.504999999999995</v>
+        <v>1</v>
       </c>
       <c r="E74">
         <v>0</v>
@@ -4446,7 +4446,7 @@
         <v>0</v>
       </c>
       <c r="G74">
-        <v>2510.495</v>
+        <v>2516</v>
       </c>
     </row>
     <row r="75">
@@ -4457,7 +4457,7 @@
         <v>1</v>
       </c>
       <c r="C75">
-        <v>0.5049999999999955</v>
+        <v>1</v>
       </c>
       <c r="D75">
         <v>1</v>
@@ -4469,7 +4469,7 @@
         <v>0</v>
       </c>
       <c r="G75">
-        <v>2512.495</v>
+        <v>2518</v>
       </c>
     </row>
     <row r="76">
@@ -4477,10 +4477,10 @@
         <v>2098</v>
       </c>
       <c r="B76">
-        <v>0.5049999999999955</v>
+        <v>1</v>
       </c>
       <c r="C76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D76">
         <v>1</v>
@@ -4492,7 +4492,7 @@
         <v>0</v>
       </c>
       <c r="G76">
-        <v>2514</v>
+        <v>2520</v>
       </c>
     </row>
     <row r="77">
@@ -4500,10 +4500,10 @@
         <v>2099</v>
       </c>
       <c r="B77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C77">
-        <v>0.5049999999999955</v>
+        <v>1</v>
       </c>
       <c r="D77">
         <v>1</v>
@@ -4515,7 +4515,7 @@
         <v>0</v>
       </c>
       <c r="G77">
-        <v>2514.99</v>
+        <v>2521</v>
       </c>
     </row>
     <row r="78">
@@ -4526,7 +4526,7 @@
         <v>0</v>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D78">
         <v>1</v>
@@ -4538,7 +4538,7 @@
         <v>0</v>
       </c>
       <c r="G78">
-        <v>2516</v>
+        <v>2522</v>
       </c>
     </row>
     <row r="79">
@@ -4549,10 +4549,10 @@
         <v>0</v>
       </c>
       <c r="C79">
-        <v>0.5049999999999955</v>
+        <v>0</v>
       </c>
       <c r="D79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E79">
         <v>0</v>
@@ -4561,7 +4561,7 @@
         <v>0</v>
       </c>
       <c r="G79">
-        <v>2516.495</v>
+        <v>2523</v>
       </c>
     </row>
     <row r="80">
@@ -4572,10 +4572,10 @@
         <v>0</v>
       </c>
       <c r="C80">
-        <v>0.5049999999999955</v>
+        <v>0</v>
       </c>
       <c r="D80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E80">
         <v>0</v>
@@ -4584,7 +4584,7 @@
         <v>0</v>
       </c>
       <c r="G80">
-        <v>2517.495</v>
+        <v>2524</v>
       </c>
     </row>
     <row r="81">
@@ -4607,7 +4607,7 @@
         <v>0</v>
       </c>
       <c r="G81">
-        <v>2517.495</v>
+        <v>2524</v>
       </c>
     </row>
     <row r="82">
@@ -4630,7 +4630,7 @@
         <v>0</v>
       </c>
       <c r="G82">
-        <v>2517.495</v>
+        <v>2525</v>
       </c>
     </row>
     <row r="83">
@@ -4653,7 +4653,7 @@
         <v>0</v>
       </c>
       <c r="G83">
-        <v>2518</v>
+        <v>2525</v>
       </c>
     </row>
     <row r="84">
@@ -4676,7 +4676,7 @@
         <v>0</v>
       </c>
       <c r="G84">
-        <v>2518.495</v>
+        <v>2525</v>
       </c>
     </row>
     <row r="85">
@@ -4699,7 +4699,7 @@
         <v>0</v>
       </c>
       <c r="G85">
-        <v>2518.495</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="86">
@@ -4722,7 +4722,7 @@
         <v>0</v>
       </c>
       <c r="G86">
-        <v>2518.495</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="87">
@@ -4736,7 +4736,7 @@
         <v>0</v>
       </c>
       <c r="D87">
-        <v>0.5049999999999955</v>
+        <v>0</v>
       </c>
       <c r="E87">
         <v>0</v>
@@ -4745,7 +4745,7 @@
         <v>0</v>
       </c>
       <c r="G87">
-        <v>2518.495</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="88">
@@ -4768,7 +4768,7 @@
         <v>0</v>
       </c>
       <c r="G88">
-        <v>2519</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="89">
@@ -4791,7 +4791,7 @@
         <v>0</v>
       </c>
       <c r="G89">
-        <v>2519.495</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="90">
@@ -4814,7 +4814,7 @@
         <v>0</v>
       </c>
       <c r="G90">
-        <v>2519.495</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="91">
@@ -4837,7 +4837,7 @@
         <v>0</v>
       </c>
       <c r="G91">
-        <v>2519.495</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="92">
@@ -4860,7 +4860,7 @@
         <v>0</v>
       </c>
       <c r="G92">
-        <v>2520</v>
+        <v>2527</v>
       </c>
     </row>
     <row r="93">
@@ -4883,7 +4883,7 @@
         <v>0</v>
       </c>
       <c r="G93">
-        <v>2520</v>
+        <v>2527</v>
       </c>
     </row>
     <row r="94">
@@ -4906,7 +4906,7 @@
         <v>0</v>
       </c>
       <c r="G94">
-        <v>2520</v>
+        <v>2527</v>
       </c>
     </row>
     <row r="95">
@@ -4929,7 +4929,7 @@
         <v>0</v>
       </c>
       <c r="G95">
-        <v>2520</v>
+        <v>2527</v>
       </c>
     </row>
     <row r="96">
@@ -4952,7 +4952,7 @@
         <v>0</v>
       </c>
       <c r="G96">
-        <v>2520</v>
+        <v>2527</v>
       </c>
     </row>
     <row r="97">
@@ -4975,7 +4975,7 @@
         <v>0</v>
       </c>
       <c r="G97">
-        <v>2520</v>
+        <v>2527</v>
       </c>
     </row>
     <row r="98">
@@ -4998,7 +4998,7 @@
         <v>0</v>
       </c>
       <c r="G98">
-        <v>2520</v>
+        <v>2527</v>
       </c>
     </row>
     <row r="99">
@@ -5021,7 +5021,7 @@
         <v>0</v>
       </c>
       <c r="G99">
-        <v>2520</v>
+        <v>2527</v>
       </c>
     </row>
     <row r="100">
@@ -5044,7 +5044,7 @@
         <v>0</v>
       </c>
       <c r="G100">
-        <v>2520</v>
+        <v>2527</v>
       </c>
     </row>
     <row r="101">
@@ -5067,7 +5067,7 @@
         <v>0</v>
       </c>
       <c r="G101">
-        <v>2520</v>
+        <v>2527</v>
       </c>
     </row>
     <row r="102">
@@ -5090,7 +5090,7 @@
         <v>0</v>
       </c>
       <c r="G102">
-        <v>2520</v>
+        <v>2527</v>
       </c>
     </row>
   </sheetData>
@@ -5120,26 +5120,26 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>10309516443.04382</v>
+        <v>9911477095.137501</v>
       </c>
       <c r="B2">
-        <v>1430785592.4583</v>
+        <v>1545014450.680892</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>705903958.0409751</v>
+        <v>753980457.850795</v>
       </c>
       <c r="B3">
-        <v>470814652.9509444</v>
+        <v>551536667.9897863</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>43699399.92867308</v>
+        <v>50196272.07274567</v>
       </c>
       <c r="B4">
-        <v>322116297.8682818</v>
+        <v>371888977.3368493</v>
       </c>
     </row>
     <row r="5">
@@ -5147,7 +5147,7 @@
         <v>0</v>
       </c>
       <c r="B5">
-        <v>1771274080.308498</v>
+        <v>1662320974.810115</v>
       </c>
     </row>
     <row r="6">
@@ -5155,7 +5155,7 @@
         <v>0</v>
       </c>
       <c r="B6">
-        <v>5267974966.728839</v>
+        <v>4001543054.391112</v>
       </c>
     </row>
   </sheetData>
@@ -5185,26 +5185,26 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>10288332451.40849</v>
+        <v>10675546796.79116</v>
       </c>
       <c r="B2">
-        <v>1530383216.837375</v>
+        <v>1348966434.759405</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>725896924.7885396</v>
+        <v>679104879.4589957</v>
       </c>
       <c r="B3">
-        <v>499536390.0530306</v>
+        <v>416226547.6455876</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>45166432.56363814</v>
+        <v>40069722.62353651</v>
       </c>
       <c r="B4">
-        <v>350552328.8269059</v>
+        <v>281336296.8027304</v>
       </c>
     </row>
     <row r="5">
@@ -5212,7 +5212,7 @@
         <v>0</v>
       </c>
       <c r="B5">
-        <v>1749705229.352344</v>
+        <v>1838289238.131983</v>
       </c>
     </row>
     <row r="6">
@@ -5220,7 +5220,7 @@
         <v>0</v>
       </c>
       <c r="B6">
-        <v>5329284428.312433</v>
+        <v>6562158177.806801</v>
       </c>
     </row>
   </sheetData>

</xml_diff>